<commit_message>
Adding more counter information in Data. Edits and additions to Intro and motivation.
</commit_message>
<xml_diff>
--- a/Data/HW_Counters.xlsx
+++ b/Data/HW_Counters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-460" windowWidth="51200" windowHeight="28800" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="51200" windowHeight="28340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PM_CMPLU_STALL_DCACHE_MISS" sheetId="1" r:id="rId1"/>
@@ -4893,7 +4893,7 @@
   <dimension ref="A1:B144"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:B84"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>